<commit_message>
Switched input and output
</commit_message>
<xml_diff>
--- a/assets/tables/booster/measurements.xlsx
+++ b/assets/tables/booster/measurements.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbr01458/GITREPO/architolk.github.io/assets/tables/booster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C77C38CD-0A85-1040-BDF7-50D391E80205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E80AA9-1956-4A4E-9D30-12D9719508BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{6422A4FA-CFD9-634E-A502-E3292F138BE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Vcc</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>D352</t>
+  </si>
+  <si>
+    <t>OC140 sec</t>
   </si>
 </sst>
 </file>
@@ -87,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,7 +123,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF817DA7-5B54-FC49-925A-B1CD26E1E957}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,7 +452,7 @@
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -465,8 +468,11 @@
       <c r="F1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -485,8 +491,11 @@
       <c r="F2">
         <v>9.1300000000000008</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>9.1300000000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -505,8 +514,11 @@
       <c r="F3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -525,8 +537,11 @@
       <c r="F4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -545,8 +560,11 @@
       <c r="F5">
         <v>1.17</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -565,8 +583,11 @@
       <c r="F6">
         <v>2160</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -585,8 +606,11 @@
       <c r="F7">
         <v>2022000</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>2022000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -610,8 +634,13 @@
         <f>1000000*F4/F6</f>
         <v>277.77777777777777</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <f>1000000*H4/H6</f>
+        <v>245.37037037037038</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -635,8 +664,13 @@
         <f>(F5-F4)/(F10*F6)</f>
         <v>59.090070136581751</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" s="3">
+        <f>(H5-H4)/(H10*H6)</f>
+        <v>44.576719576719562</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -660,8 +694,12 @@
         <f>(F2-F3)/F7</f>
         <v>4.4658753709198821E-6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <f>(H2-H3)/H7</f>
+        <v>4.4658753709198821E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -685,6 +723,11 @@
         <f>F10*1000000</f>
         <v>4.465875370919882</v>
       </c>
+      <c r="H11" s="2">
+        <f>H10*1000000</f>
+        <v>4.465875370919882</v>
+      </c>
+      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>